<commit_message>
Nova versao avisa envio
</commit_message>
<xml_diff>
--- a/public/import_tpl/import_order.xlsx
+++ b/public/import_tpl/import_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dilsonlana/Documents/workspace/avisaenvio/public/import_tpl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69133A85-4262-E240-A3D9-E55363A56F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2B9474-3B24-BF48-BDB8-2EDA432C99DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1880" windowWidth="28040" windowHeight="16900" xr2:uid="{654BC871-05DC-5840-B76F-4CD9EB7BF628}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>WHATSAPP (DDD + DDI + NÚMERO)</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>DESTINATÁRIO</t>
+  </si>
+  <si>
+    <t>CPF/CNPJ</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D49CF9-1596-C04B-808E-85D157E10950}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -439,24 +442,27 @@
     <col min="1" max="1" width="47.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="36.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>

</xml_diff>